<commit_message>
vistas html de mis grupos y de reportes diarios
</commit_message>
<xml_diff>
--- a/recursos/documentos/spintUno/BaseDatos_16-06-2022.xlsx
+++ b/recursos/documentos/spintUno/BaseDatos_16-06-2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Equipo5\proyectoEquipo5\recursos\documentos\spintUno\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
-    <t>daily_usuarios</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>usuarios</t>
   </si>
   <si>
-    <t xml:space="preserve">daily </t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>Faúndez</t>
   </si>
   <si>
-    <t>grupo</t>
-  </si>
-  <si>
     <t>grupos_usuarios</t>
   </si>
   <si>
@@ -141,6 +132,15 @@
   </si>
   <si>
     <t xml:space="preserve">grupo scrum </t>
+  </si>
+  <si>
+    <t>grupos</t>
+  </si>
+  <si>
+    <t>dailys</t>
+  </si>
+  <si>
+    <t>dailys_usuarios</t>
   </si>
 </sst>
 </file>
@@ -277,15 +277,6 @@
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -310,6 +301,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,19 +347,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,12 +363,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -904,7 +904,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,364 +916,364 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="11" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="K8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="26"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="K8" s="17" t="s">
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="H9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="K9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="M9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="20" t="s">
+      <c r="N9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>1</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="E10" s="12">
+        <v>34367</v>
+      </c>
+      <c r="F10" s="10">
+        <v>28</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="H10" s="10">
+        <v>123345</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1</v>
+      </c>
+      <c r="L10" s="12">
+        <v>44727</v>
+      </c>
+      <c r="M10" s="14">
+        <v>1</v>
+      </c>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="21">
-        <v>34367</v>
-      </c>
-      <c r="F10" s="13">
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="K11" s="10">
+        <v>2</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="K12" s="10">
+        <v>3</v>
+      </c>
+      <c r="L12" s="10"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>4</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="13">
-        <v>123345</v>
-      </c>
-      <c r="K10" s="8">
-        <v>1</v>
-      </c>
-      <c r="L10" s="21">
-        <v>44727</v>
-      </c>
-      <c r="M10" s="23">
-        <v>1</v>
-      </c>
-      <c r="N10" s="11"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="C13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>5</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J16" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+      <c r="J17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F18" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="K11" s="13">
+      <c r="J18" s="14">
+        <v>1</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="17">
+        <v>1</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="J19" s="16">
         <v>2</v>
       </c>
-      <c r="L11" s="13"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="K19" s="16"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="10">
+        <v>2</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
+      <c r="H20" s="10">
+        <v>2</v>
+      </c>
+      <c r="J20" s="16">
         <v>3</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="K12" s="13">
+      <c r="K20" s="16"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="10">
         <v>3</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="G21" s="10">
+        <v>1</v>
+      </c>
+      <c r="H21" s="10">
+        <v>3</v>
+      </c>
+      <c r="J21" s="10">
         <v>4</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="K21" s="10"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="10">
+        <v>4</v>
+      </c>
+      <c r="G22" s="10">
+        <v>1</v>
+      </c>
+      <c r="H22" s="10">
+        <v>4</v>
+      </c>
+      <c r="J22" s="10">
         <v>5</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J16" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
-    </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F17" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="J17" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F18" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" s="23">
-        <v>1</v>
-      </c>
-      <c r="K18" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="32">
-        <v>1</v>
-      </c>
-      <c r="G19" s="23">
-        <v>1</v>
-      </c>
-      <c r="H19" s="9">
-        <v>1</v>
-      </c>
-      <c r="J19" s="31">
-        <v>2</v>
-      </c>
-      <c r="K19" s="31"/>
-      <c r="L19" s="11"/>
-    </row>
-    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="13">
-        <v>2</v>
-      </c>
-      <c r="G20" s="13">
-        <v>1</v>
-      </c>
-      <c r="H20" s="13">
-        <v>2</v>
-      </c>
-      <c r="J20" s="31">
-        <v>3</v>
-      </c>
-      <c r="K20" s="31"/>
-      <c r="L20" s="11"/>
-    </row>
-    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="13">
-        <v>3</v>
-      </c>
-      <c r="G21" s="13">
-        <v>1</v>
-      </c>
-      <c r="H21" s="13">
-        <v>3</v>
-      </c>
-      <c r="J21" s="13">
-        <v>4</v>
-      </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="11"/>
-    </row>
-    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F22" s="13">
-        <v>4</v>
-      </c>
-      <c r="G22" s="13">
-        <v>1</v>
-      </c>
-      <c r="H22" s="13">
-        <v>4</v>
-      </c>
-      <c r="J22" s="13">
+      <c r="K22" s="10"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F23" s="10">
         <v>5</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="11"/>
-    </row>
-    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F23" s="13">
+      <c r="G23" s="10">
+        <v>1</v>
+      </c>
+      <c r="H23" s="10">
         <v>5</v>
       </c>
-      <c r="G23" s="13">
-        <v>1</v>
-      </c>
-      <c r="H23" s="13">
-        <v>5</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>